<commit_message>
reorg to match /orange directories
</commit_message>
<xml_diff>
--- a/sample_annotation_busco.xlsx
+++ b/sample_annotation_busco.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uflorida-my.sharepoint.com/personal/kasey_pham_ufl_edu/Documents/Grad School Documents/Projects/nitfix/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uflorida-my.sharepoint.com/personal/kasey_pham_ufl_edu/Documents/Grad School Documents/Projects/nitfix-annotation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="116" documentId="11_F25DC773A252ABDACC1048CC295F61E45BDE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{395CAC4E-FCA5-470B-86DC-F6530D51242C}"/>
+  <xr:revisionPtr revIDLastSave="192" documentId="11_F25DC773A252ABDACC1048CC295F61E45BDE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74F26B16-9427-4AAE-A170-BB8181C3CD25}"/>
   <bookViews>
-    <workbookView xWindow="-21840" yWindow="-8115" windowWidth="15000" windowHeight="12585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1308" yWindow="-108" windowWidth="21840" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Our genomes" sheetId="1" r:id="rId1"/>
+    <sheet name="Publically available" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="54">
   <si>
     <t>Taxon</t>
   </si>
@@ -48,9 +49,6 @@
     <t>Ceanothus americanus</t>
   </si>
   <si>
-    <t>Corynocarpus laevigatus</t>
-  </si>
-  <si>
     <t>Corynocarpus_laevigatus_final.fa</t>
   </si>
   <si>
@@ -139,6 +137,57 @@
   </si>
   <si>
     <t>WVEF-translated-nucleotides.fa</t>
+  </si>
+  <si>
+    <t>Sageretia minutiflora</t>
+  </si>
+  <si>
+    <t>Tetrameles nudiflora</t>
+  </si>
+  <si>
+    <t>Tetra_nudifolius.final.fa</t>
+  </si>
+  <si>
+    <t>Sageretia.final.fa</t>
+  </si>
+  <si>
+    <t>Begonia sp.</t>
+  </si>
+  <si>
+    <t>OCTM-translated-nucleotides.fa</t>
+  </si>
+  <si>
+    <t>Canicomyrica</t>
+  </si>
+  <si>
+    <t>Fixer/Non-fixer</t>
+  </si>
+  <si>
+    <t>Fixer</t>
+  </si>
+  <si>
+    <t>Non-fixer</t>
+  </si>
+  <si>
+    <t>Purshia</t>
+  </si>
+  <si>
+    <t>Datisca</t>
+  </si>
+  <si>
+    <t>Outgroup</t>
+  </si>
+  <si>
+    <t>Dryas</t>
+  </si>
+  <si>
+    <t>Neillia sinensis</t>
+  </si>
+  <si>
+    <t>Corynocarpus laevigatus*</t>
+  </si>
+  <si>
+    <t>Coriaria nepalensis*</t>
   </si>
 </sst>
 </file>
@@ -162,12 +211,42 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -182,9 +261,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,214 +549,357 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="H1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2">
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2">
         <v>85.4</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>89.9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3">
+        <v>78.599999999999994</v>
+      </c>
+      <c r="G3">
+        <v>95.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4">
+        <v>69</v>
+      </c>
+      <c r="G4">
+        <v>80.400000000000006</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
         <v>21</v>
       </c>
-      <c r="E3">
-        <v>78.599999999999994</v>
-      </c>
-      <c r="F3">
-        <v>95.8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4">
-        <v>69</v>
-      </c>
-      <c r="F4">
-        <v>80.400000000000006</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5">
+        <v>70.3</v>
+      </c>
+      <c r="G5">
+        <v>82.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5">
-        <v>70.3</v>
-      </c>
-      <c r="F5">
-        <v>82.1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="B6" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6">
+        <v>80.099999999999994</v>
+      </c>
+      <c r="G6">
+        <v>86.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" t="s">
         <v>15</v>
       </c>
-      <c r="E6">
-        <v>80.099999999999994</v>
-      </c>
-      <c r="F6">
-        <v>86.2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
       <c r="D7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7">
         <v>78.099999999999994</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" t="s">
-        <v>26</v>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="C8" t="s">
         <v>25</v>
       </c>
       <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8">
+        <v>74.099999999999994</v>
+      </c>
+      <c r="G8">
+        <v>84.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
         <v>31</v>
       </c>
-      <c r="E8">
-        <v>74.099999999999994</v>
-      </c>
-      <c r="F8">
-        <v>84.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="E9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9">
+        <v>87.2</v>
+      </c>
+      <c r="G9">
+        <v>90.7</v>
+      </c>
+      <c r="H9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" t="s">
-        <v>30</v>
+      <c r="B10" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="C10" t="s">
         <v>29</v>
       </c>
       <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10">
+        <v>88.2</v>
+      </c>
+      <c r="G10">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
         <v>37</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6780D4C5-2639-4B06-AC35-8EBA913EA872}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B2:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="5"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>